<commit_message>
Fix typos in Emma's hand-disambiguation
</commit_message>
<xml_diff>
--- a/analyses/4-record-sampling-analysis/2022-07-25-Emma-patent-samples-part-2.xlsx
+++ b/analyses/4-record-sampling-analysis/2022-07-25-Emma-patent-samples-part-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25524"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msair-my.sharepoint.com/personal/ehickerson_air_org/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{747A0FA7-9B16-44C0-AE8B-ADDC56C3656C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF759115-3071-497B-B69E-F6BCEC12DDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="660" windowWidth="16440" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="880">
   <si>
     <t>patent_id</t>
   </si>
@@ -121,7 +121,7 @@
     <t>Erman</t>
   </si>
   <si>
-    <t>US8561841-6, US7475795-4, US9296603-1,US9738507-1</t>
+    <t>US8561841-0, US7475795-3, US9296603-1,US9738507-1</t>
   </si>
   <si>
     <t>fl:to_ln:geniesse-1</t>
@@ -190,7 +190,7 @@
     <t>Rogers</t>
   </si>
   <si>
-    <t>US10916408-3, US10923321-3, US11049760-2, US10991556-4</t>
+    <t>US10916408-2, US10923321-3, US11049760-3, US10991556-4</t>
   </si>
   <si>
     <t>US6027337-0, US4233600-0, US5372255-1, US5069513-1, US5395467-0, US5102482-0, US3952855-0, US8038436-0, US4023666-0, US10375884-1</t>
@@ -211,7 +211,7 @@
     <t>Schaffner</t>
   </si>
   <si>
-    <t>US7182369-5, US6726436-5, US7390021-5</t>
+    <t>US7182369-4, US6726436-4, US7390021-4</t>
   </si>
   <si>
     <t>D784389</t>
@@ -226,7 +226,7 @@
     <t>Kim</t>
   </si>
   <si>
-    <t xml:space="preserve">USD815134-0, USD822698-0, USD852212-0, USD849019-0, USD874496-1, USD808409-0, USD876458-1, USD868810-1, USD868089-1, USD851107-0, USD756394-0, USD898052-1, USD919644-1, USD876459-1, USD897358-1, USD916848-1, USD897360-1, USD897359-1, USD921657-1, USD919643-1, USD873841-0, USD811435-1, US9977523-0, USD915432-1, USD892146-0, USD747332-0, USD741888-0, USD736241-0, USD734766-0, USD751591-0, USD746841-0, US10560576-2, US9939937-0, USD931888-1, USD937292-0, USD936092-1, USD931301-1
+    <t xml:space="preserve">USD815134-0, USD822698-0, USD852212-0, USD849019-0, USD874496-1, USD808409-0, USD876458-1, USD868810-1, USD868089-1, USD851107-0, USD756394-0, USD898052-1, USD919644-1, USD876459-1, USD897358-1, USD916848-1, USD897360-1, USD897359-1, USD921657-1, USD919643-1, USD873841-0, USD811435-1, US9977523-0, USD915432-1, USD892146-0, USD747332-0, USD741888-0, USD736241-0, USD734766-1, USD751591-0, USD746841-0, US10560576-2, US9939937-0, USD931888-1, USD937292-0, USD936092-1, USD931301-1
 </t>
   </si>
   <si>
@@ -257,7 +257,7 @@
     <t>Droz</t>
   </si>
   <si>
-    <t>US10971645-0, US10967856-0, US11041753-1, US10942272-1, US10976437-5, US10971787-1, US10989886-0, US11042004-0, US10942244-0, US11016180-0, US11029396-0, US11042164-2, US10962883-1, US10884115-1, US10890650-2, US10948573-1</t>
+    <t>US10971645-2, US10967856-0, US11041753-0, US10942272-0, US10976437-5, US10971787-0, US10989886-0, US11042004-1, US10942244-0, US11016180-2, US11029396-0, US11042164-1, US10962883-1, US10884115-3, US10890650-0, US10948573-1</t>
   </si>
   <si>
     <t>waymo and apple</t>
@@ -272,10 +272,13 @@
     <t>Vembu</t>
   </si>
   <si>
-    <t>US10956223-1, US10955896-2, US10936214-2, US10963986-4, US10977762-2, US10896479-2, US10901909-6, US10908865-19, US11048605-7, US10922869-7</t>
+    <t>US10956223-1, US10955896-7, US10936214-6, US10963986-0, US10977762-0, US10896479-0, US10901909-3, US10908865-13, US11048605-1, US10922869-0</t>
   </si>
   <si>
     <t>unsure if anything needs to be removed. Some assignees as McAfee which is not on his linkedin but is computer related</t>
+  </si>
+  <si>
+    <t>sequence numbers were wrong</t>
   </si>
   <si>
     <t>fl:ro_ln:tsai-10</t>
@@ -846,7 +849,7 @@
     <t>Verlinden</t>
   </si>
   <si>
-    <t>US6366013-1, US6074110-0, US6309901-1, US6092392-0, US6861136-0, US5871879-0, US6306510-0, US5652939-0, US5745816-0, US5771090-0, US5568693-3, US5561027-0, US5530511-0, US5737662-0, US7837298-3, US5899595-0, US6102588-0, US5689750-0, US5861236-0, US6250222-0, US6071020-0, US5720840-1, US6049344-0, US5448325-0, US6197418-3, US6131512-0, US6120907-1, US5188732-3, US5133846-4, US5118402-2, US7032520-0</t>
+    <t>US6366013-1, US6074110-0, US6309901-1, US6092392-0, US6861136-0, US5871879-0, US6306510-0, US5652939-0, US5745816-0, US5771090-0, US5568693-3, US5561027-0, US5530511-0, US5737662-0, US7837298-3, US5899595-0, US6102588-0, US5689750-0, US5861236-0, US6250222-0, US6071020-0, US5720840-1, US6049344-0, US5448325-0, US6197418-3, US6131512-0, US6120907-1, US5188732-3, US5133846-4, US5118402-2, US7032520-2</t>
   </si>
   <si>
     <t>US8099884-1</t>
@@ -3081,16 +3084,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I201"/>
+  <dimension ref="A1:J201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F163" sqref="F163"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" customWidth="1"/>
@@ -3448,7 +3451,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="152.25">
+    <row r="17" spans="1:10" ht="152.25">
       <c r="A17">
         <v>10403003</v>
       </c>
@@ -3470,42 +3473,45 @@
       <c r="I17" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="45.75">
+      <c r="J17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45.75">
       <c r="A18">
         <v>7800132</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15">
       <c r="A19">
         <v>7346888</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -3514,18 +3520,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15">
+    <row r="20" spans="1:10" ht="15">
       <c r="A20">
         <v>6037233</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -3534,41 +3540,41 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="105" customHeight="1">
+    <row r="21" spans="1:10" ht="105" customHeight="1">
       <c r="A21">
         <v>7722378</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D22" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -3577,18 +3583,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15">
+    <row r="23" spans="1:10" ht="15">
       <c r="A23">
         <v>9077995</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D23" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E23">
         <v>3</v>
@@ -3597,18 +3603,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15">
+    <row r="24" spans="1:10" ht="15">
       <c r="A24">
         <v>5384075</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -3617,18 +3623,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15">
+    <row r="25" spans="1:10" ht="15">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E25">
         <v>5</v>
@@ -3637,21 +3643,21 @@
         <v>12</v>
       </c>
       <c r="I25" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D26" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -3660,18 +3666,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15">
+    <row r="27" spans="1:10" ht="15">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -3680,41 +3686,41 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="409.6">
+    <row r="28" spans="1:10" ht="409.6">
       <c r="A28">
         <v>8018561</v>
       </c>
       <c r="B28" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D28" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15">
       <c r="A29">
         <v>7893713</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C29" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -3723,18 +3729,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15">
+    <row r="30" spans="1:10" ht="15">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D30" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -3743,18 +3749,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15">
+    <row r="31" spans="1:10" ht="15">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C31" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -3763,18 +3769,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15">
+    <row r="32" spans="1:10" ht="15">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E32">
         <v>6</v>
@@ -3785,16 +3791,16 @@
     </row>
     <row r="33" spans="1:8" ht="15">
       <c r="A33" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B33" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D33" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -3805,36 +3811,36 @@
     </row>
     <row r="34" spans="1:8" ht="15">
       <c r="A34" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C34" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D34" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B35" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C35" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D35" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E35">
         <v>5</v>
@@ -3845,16 +3851,16 @@
     </row>
     <row r="36" spans="1:8" ht="15">
       <c r="A36" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B36" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C36" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D36" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E36">
         <v>4</v>
@@ -3868,33 +3874,33 @@
         <v>10578479</v>
       </c>
       <c r="B37" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D37" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15">
       <c r="A38" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B38" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C38" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D38" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -3905,16 +3911,16 @@
     </row>
     <row r="39" spans="1:8" ht="15">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B39" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C39" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D39" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -3925,16 +3931,16 @@
     </row>
     <row r="40" spans="1:8" ht="15">
       <c r="A40" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B40" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C40" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D40" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E40">
         <v>2</v>
@@ -3945,16 +3951,16 @@
     </row>
     <row r="41" spans="1:8" ht="15">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B41" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C41" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D41" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -3965,16 +3971,16 @@
     </row>
     <row r="42" spans="1:8" ht="15">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B42" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C42" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D42" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E42">
         <v>5</v>
@@ -3988,36 +3994,36 @@
         <v>10647081</v>
       </c>
       <c r="B43" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C43" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D43" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15">
       <c r="A44" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B44" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C44" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D44" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -4028,36 +4034,36 @@
     </row>
     <row r="45" spans="1:8" ht="409.6">
       <c r="A45" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B45" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C45" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D45" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15">
       <c r="A46" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B46" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C46" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D46" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -4068,16 +4074,16 @@
     </row>
     <row r="47" spans="1:8" ht="15">
       <c r="A47" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B47" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C47" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D47" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -4088,16 +4094,16 @@
     </row>
     <row r="48" spans="1:8" ht="15">
       <c r="A48" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B48" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C48" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D48" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -4108,16 +4114,16 @@
     </row>
     <row r="49" spans="1:8" ht="15">
       <c r="A49" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B49" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C49" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D49" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -4128,16 +4134,16 @@
     </row>
     <row r="50" spans="1:8" ht="15">
       <c r="A50" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B50" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C50" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D50" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -4148,16 +4154,16 @@
     </row>
     <row r="51" spans="1:8" ht="15">
       <c r="A51" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B51" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C51" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D51" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -4168,16 +4174,16 @@
     </row>
     <row r="52" spans="1:8" ht="15">
       <c r="A52" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B52" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C52" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D52" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E52">
         <v>3</v>
@@ -4188,16 +4194,16 @@
     </row>
     <row r="53" spans="1:8" ht="15">
       <c r="A53" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B53" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C53" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D53" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E53">
         <v>2</v>
@@ -4208,36 +4214,36 @@
     </row>
     <row r="54" spans="1:8" ht="91.5">
       <c r="A54" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B54" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C54" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D54" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15">
       <c r="A55" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B55" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C55" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D55" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E55">
         <v>9</v>
@@ -4248,16 +4254,16 @@
     </row>
     <row r="56" spans="1:8" ht="15">
       <c r="A56" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B56" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C56" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D56" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E56">
         <v>3</v>
@@ -4268,36 +4274,36 @@
     </row>
     <row r="57" spans="1:8" ht="103.5" customHeight="1">
       <c r="A57" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B57" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C57" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D57" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E57">
         <v>1</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15">
       <c r="A58" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B58" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C58" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D58" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -4308,16 +4314,16 @@
     </row>
     <row r="59" spans="1:8" ht="15">
       <c r="A59" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B59" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C59" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D59" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -4328,16 +4334,16 @@
     </row>
     <row r="60" spans="1:8" ht="15">
       <c r="A60" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B60" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C60" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D60" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E60">
         <v>23</v>
@@ -4348,36 +4354,36 @@
     </row>
     <row r="61" spans="1:8" ht="15">
       <c r="A61" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B61" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C61" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D61" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E61">
         <v>2</v>
       </c>
       <c r="G61" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="15">
       <c r="A62" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B62" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C62" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D62" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -4388,39 +4394,39 @@
     </row>
     <row r="63" spans="1:8" ht="244.5">
       <c r="A63" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B63" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C63" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D63" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15">
       <c r="A64" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B64" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C64" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D64" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E64">
         <v>2</v>
@@ -4431,39 +4437,39 @@
     </row>
     <row r="65" spans="1:9" ht="60.75">
       <c r="A65" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B65" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C65" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D65" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E65">
         <v>6</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="I65" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="15">
       <c r="A66" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B66" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C66" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D66" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E66">
         <v>5</v>
@@ -4474,16 +4480,16 @@
     </row>
     <row r="67" spans="1:9" ht="15">
       <c r="A67" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B67" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C67" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D67" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E67">
         <v>2</v>
@@ -4494,16 +4500,16 @@
     </row>
     <row r="68" spans="1:9" ht="15">
       <c r="A68" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B68" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C68" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D68" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E68">
         <v>5</v>
@@ -4514,16 +4520,16 @@
     </row>
     <row r="69" spans="1:9" ht="15">
       <c r="A69" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B69" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C69" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D69" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E69">
         <v>5</v>
@@ -4537,79 +4543,79 @@
         <v>6069575</v>
       </c>
       <c r="B70" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C70" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D70" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E70">
         <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="I70" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="45.75">
       <c r="A71" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B71" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C71" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D71" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E71">
         <v>10</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="15">
       <c r="A72" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B72" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C72" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D72" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="15">
       <c r="A73" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B73" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C73" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D73" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -4620,16 +4626,16 @@
     </row>
     <row r="74" spans="1:9" ht="15">
       <c r="A74" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B74" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C74" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D74" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E74">
         <v>2</v>
@@ -4640,56 +4646,56 @@
     </row>
     <row r="75" spans="1:9" ht="15">
       <c r="A75" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B75" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C75" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D75" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E75">
         <v>2</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="106.5">
       <c r="A76" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B76" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C76" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D76" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E76">
         <v>0</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="15">
       <c r="A77" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B77" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C77" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D77" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -4700,36 +4706,36 @@
     </row>
     <row r="78" spans="1:9" ht="409.6">
       <c r="A78" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B78" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C78" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D78" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="15">
       <c r="A79" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B79" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C79" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D79" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -4740,36 +4746,36 @@
     </row>
     <row r="80" spans="1:9" ht="121.5">
       <c r="A80" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B80" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C80" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D80" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E80">
         <v>2</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="15">
       <c r="A81" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B81" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C81" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D81" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -4780,16 +4786,16 @@
     </row>
     <row r="82" spans="1:9" ht="15">
       <c r="A82" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B82" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C82" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D82" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -4800,16 +4806,16 @@
     </row>
     <row r="83" spans="1:9" ht="15">
       <c r="A83" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B83" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C83" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D83" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -4820,108 +4826,108 @@
     </row>
     <row r="84" spans="1:9" ht="15">
       <c r="A84" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B84" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C84" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D84" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="G84" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="91.5">
       <c r="A85" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B85" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C85" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D85" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="I85" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="409.6">
       <c r="A86" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B86" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C86" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D86" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E86">
         <v>2</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="I86" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="15">
       <c r="A87" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B87" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C87" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D87" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E87">
         <v>1</v>
       </c>
       <c r="G87" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="I87" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="15">
       <c r="A88" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B88" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C88" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D88" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E88">
         <v>2</v>
@@ -4932,13 +4938,13 @@
     </row>
     <row r="89" spans="1:9" ht="15">
       <c r="A89" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B89" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C89" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D89" t="s">
         <v>63</v>
@@ -4952,16 +4958,16 @@
     </row>
     <row r="90" spans="1:9" ht="15">
       <c r="A90" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B90" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C90" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D90" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -4972,16 +4978,16 @@
     </row>
     <row r="91" spans="1:9" ht="15">
       <c r="A91" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B91" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C91" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D91" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -4992,16 +4998,16 @@
     </row>
     <row r="92" spans="1:9" ht="15">
       <c r="A92" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B92" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C92" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D92" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -5012,16 +5018,16 @@
     </row>
     <row r="93" spans="1:9" ht="15">
       <c r="A93" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B93" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C93" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D93" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -5032,16 +5038,16 @@
     </row>
     <row r="94" spans="1:9" ht="15">
       <c r="A94" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B94" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C94" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D94" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E94">
         <v>0</v>
@@ -5052,16 +5058,16 @@
     </row>
     <row r="95" spans="1:9" ht="15">
       <c r="A95" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B95" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C95" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D95" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -5075,33 +5081,33 @@
         <v>7804358</v>
       </c>
       <c r="B96" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C96" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D96" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E96">
         <v>2</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="15">
       <c r="A97" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B97" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C97" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D97" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -5112,16 +5118,16 @@
     </row>
     <row r="98" spans="1:9" ht="15">
       <c r="A98" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B98" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C98" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D98" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E98">
         <v>5</v>
@@ -5132,16 +5138,16 @@
     </row>
     <row r="99" spans="1:9" ht="15">
       <c r="A99" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B99" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C99" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D99" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E99">
         <v>12</v>
@@ -5152,16 +5158,16 @@
     </row>
     <row r="100" spans="1:9" ht="15">
       <c r="A100" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B100" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C100" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D100" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -5172,16 +5178,16 @@
     </row>
     <row r="101" spans="1:9" ht="15">
       <c r="A101" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B101" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C101" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D101" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -5192,79 +5198,79 @@
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="3" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B102" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C102" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D102" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E102">
         <v>0</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="318.95">
       <c r="A103" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B103" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C103" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D103" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E103">
         <v>4</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="I103" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B104" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C104" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D104" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E104">
         <v>6</v>
       </c>
       <c r="G104" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B105" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C105" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D105" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -5275,16 +5281,16 @@
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B106" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C106" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D106" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E106">
         <v>0</v>
@@ -5295,16 +5301,16 @@
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B107" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C107" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D107" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -5315,16 +5321,16 @@
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B108" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C108" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D108" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E108">
         <v>0</v>
@@ -5335,16 +5341,16 @@
     </row>
     <row r="109" spans="1:9">
       <c r="A109" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B109" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C109" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D109" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E109">
         <v>2</v>
@@ -5355,83 +5361,83 @@
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B110" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C110" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D110" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E110">
         <v>3</v>
       </c>
       <c r="F110" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="377.1">
       <c r="A111" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B111" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C111" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D111" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E111">
         <v>2</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="I111" s="7"/>
     </row>
     <row r="112" spans="1:9" ht="409.5">
       <c r="A112" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B112" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C112" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D112" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E112">
         <v>1</v>
       </c>
       <c r="F112" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="I112" s="5" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B113" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C113" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D113" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E113">
         <v>2</v>
@@ -5442,16 +5448,16 @@
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B114" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C114" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D114" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E114">
         <v>1</v>
@@ -5462,16 +5468,16 @@
     </row>
     <row r="115" spans="1:9">
       <c r="A115" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B115" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C115" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D115" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="E115">
         <v>1</v>
@@ -5482,56 +5488,56 @@
     </row>
     <row r="116" spans="1:9" ht="409.5">
       <c r="A116" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B116" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C116" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D116" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E116">
         <v>2</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="409.6">
       <c r="A117" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B117" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C117" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D117" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E117">
         <v>0</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B118" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C118" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D118" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E118">
         <v>0</v>
@@ -5542,39 +5548,39 @@
     </row>
     <row r="119" spans="1:9" ht="101.45">
       <c r="A119" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B119" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C119" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D119" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E119">
         <v>0</v>
       </c>
       <c r="G119" s="9" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="I119" s="5" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B120" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C120" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D120" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E120">
         <v>0</v>
@@ -5585,16 +5591,16 @@
     </row>
     <row r="121" spans="1:9">
       <c r="A121" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B121" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C121" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D121" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E121">
         <v>2</v>
@@ -5605,16 +5611,16 @@
     </row>
     <row r="122" spans="1:9">
       <c r="A122" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B122" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C122" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D122" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E122">
         <v>1</v>
@@ -5625,16 +5631,16 @@
     </row>
     <row r="123" spans="1:9">
       <c r="A123" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B123" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C123" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D123" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E123">
         <v>1</v>
@@ -5645,36 +5651,36 @@
     </row>
     <row r="124" spans="1:9">
       <c r="A124" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B124" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C124" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D124" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E124">
         <v>1</v>
       </c>
       <c r="F124" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B125" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C125" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D125" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E125">
         <v>0</v>
@@ -5685,36 +5691,36 @@
     </row>
     <row r="126" spans="1:9">
       <c r="A126" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B126" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C126" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D126" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E126">
         <v>1</v>
       </c>
       <c r="G126" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B127" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C127" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D127" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E127">
         <v>0</v>
@@ -5725,16 +5731,16 @@
     </row>
     <row r="128" spans="1:9">
       <c r="A128" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B128" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C128" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D128" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E128">
         <v>0</v>
@@ -5745,16 +5751,16 @@
     </row>
     <row r="129" spans="1:9">
       <c r="A129" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B129" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C129" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D129" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E129">
         <v>2</v>
@@ -5765,73 +5771,73 @@
     </row>
     <row r="130" spans="1:9" ht="144.94999999999999">
       <c r="A130" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B130" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C130" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D130" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="E130">
         <v>2</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="43.5">
       <c r="A131" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B131" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C131" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="D131" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="E131">
         <v>0</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="130.5">
       <c r="A132" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B132" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C132" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="D132" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="E132">
         <v>0</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="57.95">
       <c r="A133" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B133" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C133" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="D133" t="s">
         <v>63</v>
@@ -5840,27 +5846,27 @@
         <v>1</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="G133" s="9" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="I133" s="5" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="134" spans="1:9">
       <c r="A134" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B134" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C134" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="D134" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E134">
         <v>0</v>
@@ -5871,16 +5877,16 @@
     </row>
     <row r="135" spans="1:9">
       <c r="A135" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B135" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C135" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="D135" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="E135">
         <v>1</v>
@@ -5891,16 +5897,16 @@
     </row>
     <row r="136" spans="1:9">
       <c r="A136" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B136" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C136" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D136" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="E136">
         <v>0</v>
@@ -5911,16 +5917,16 @@
     </row>
     <row r="137" spans="1:9">
       <c r="A137" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B137" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C137" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="D137" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="E137">
         <v>0</v>
@@ -5931,36 +5937,36 @@
     </row>
     <row r="138" spans="1:9" ht="29.1">
       <c r="A138" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B138" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C138" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D138" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="E138">
         <v>0</v>
       </c>
       <c r="G138" s="5" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B139" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C139" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D139" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E139">
         <v>0</v>
@@ -5971,16 +5977,16 @@
     </row>
     <row r="140" spans="1:9">
       <c r="A140" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B140" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C140" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D140" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="E140">
         <v>1</v>
@@ -5991,36 +5997,36 @@
     </row>
     <row r="141" spans="1:9" ht="87">
       <c r="A141" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B141" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C141" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D141" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="E141">
         <v>2</v>
       </c>
       <c r="G141" s="6" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B142" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C142" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D142" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="E142">
         <v>0</v>
@@ -6031,16 +6037,16 @@
     </row>
     <row r="143" spans="1:9">
       <c r="A143" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B143" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C143" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D143" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="E143">
         <v>0</v>
@@ -6051,122 +6057,122 @@
     </row>
     <row r="144" spans="1:9">
       <c r="A144" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B144" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C144" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D144" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="E144">
         <v>0</v>
       </c>
       <c r="G144" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="145" spans="1:9">
       <c r="A145" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B145" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C145" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D145" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="E145">
         <v>1</v>
       </c>
       <c r="F145" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="57.95">
       <c r="A146" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B146" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="C146" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="D146" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="E146">
         <v>1</v>
       </c>
       <c r="G146" s="5" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="I146" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="116.1">
       <c r="A147" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B147" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C147" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D147" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E147">
         <v>1</v>
       </c>
       <c r="G147" s="9" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="I147" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="362.45">
       <c r="A148" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B148" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C148" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="D148" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="E148">
         <v>0</v>
       </c>
       <c r="G148" s="5" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="149" spans="1:9">
       <c r="A149" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B149" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="C149" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D149" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="E149">
         <v>1</v>
@@ -6177,16 +6183,16 @@
     </row>
     <row r="150" spans="1:9">
       <c r="A150" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B150" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C150" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D150" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="E150">
         <v>0</v>
@@ -6197,36 +6203,36 @@
     </row>
     <row r="151" spans="1:9">
       <c r="A151" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B151" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C151" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="D151" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="E151">
         <v>0</v>
       </c>
       <c r="F151" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="152" spans="1:9">
       <c r="A152" s="3" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B152" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C152" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D152" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="E152">
         <v>0</v>
@@ -6237,96 +6243,96 @@
     </row>
     <row r="153" spans="1:9">
       <c r="A153" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B153" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C153" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D153" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="E153">
         <v>0</v>
       </c>
       <c r="G153" s="4" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="29.1">
       <c r="A154" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B154" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C154" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D154" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="E154">
         <v>1</v>
       </c>
       <c r="G154" s="9" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="72.599999999999994">
       <c r="A155" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B155" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C155" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="D155" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="E155">
         <v>1</v>
       </c>
       <c r="F155" s="5" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="156" spans="1:9">
       <c r="A156" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B156" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C156" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="D156" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="E156">
         <v>0</v>
       </c>
       <c r="F156" s="4" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="157" spans="1:9">
       <c r="A157" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B157" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="C157" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D157" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E157">
         <v>1</v>
@@ -6337,16 +6343,16 @@
     </row>
     <row r="158" spans="1:9">
       <c r="A158" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B158" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C158" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="D158" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="E158">
         <v>2</v>
@@ -6357,16 +6363,16 @@
     </row>
     <row r="159" spans="1:9">
       <c r="A159" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B159" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C159" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D159" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="E159">
         <v>2</v>
@@ -6377,36 +6383,36 @@
     </row>
     <row r="160" spans="1:9">
       <c r="A160" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B160" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C160" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="D160" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="E160">
         <v>0</v>
       </c>
       <c r="F160" s="4" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="161" spans="1:9">
       <c r="A161" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B161" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C161" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="D161" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E161">
         <v>2</v>
@@ -6417,60 +6423,60 @@
     </row>
     <row r="162" spans="1:9" ht="409.6">
       <c r="A162" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B162" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C162" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="D162" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E162">
         <v>0</v>
       </c>
       <c r="F162" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="G162" s="5" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="20.25" customHeight="1">
       <c r="A163" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B163" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C163" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="D163" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="E163">
         <v>0</v>
       </c>
       <c r="G163" s="5"/>
       <c r="I163" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="164" spans="1:9">
       <c r="A164" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B164" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C164" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D164" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="E164">
         <v>0</v>
@@ -6481,36 +6487,36 @@
     </row>
     <row r="165" spans="1:9">
       <c r="A165" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B165" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C165" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="D165" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="E165">
         <v>0</v>
       </c>
       <c r="G165" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="166" spans="1:9">
       <c r="A166" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B166" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C166" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D166" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="E166">
         <v>2</v>
@@ -6521,16 +6527,16 @@
     </row>
     <row r="167" spans="1:9">
       <c r="A167" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B167" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C167" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="D167" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="E167">
         <v>0</v>
@@ -6541,16 +6547,16 @@
     </row>
     <row r="168" spans="1:9">
       <c r="A168" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B168" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C168" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="D168" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E168">
         <v>0</v>
@@ -6561,16 +6567,16 @@
     </row>
     <row r="169" spans="1:9">
       <c r="A169" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B169" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C169" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D169" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="E169">
         <v>2</v>
@@ -6581,59 +6587,59 @@
     </row>
     <row r="170" spans="1:9" ht="57.95">
       <c r="A170" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B170" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C170" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="D170" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="E170">
         <v>2</v>
       </c>
       <c r="F170" s="5" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="144.94999999999999">
       <c r="A171" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B171" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C171" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D171" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="E171">
         <v>0</v>
       </c>
       <c r="F171" s="5" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="I171" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="172" spans="1:9">
       <c r="A172" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B172" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C172" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="D172" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="E172">
         <v>0</v>
@@ -6644,56 +6650,56 @@
     </row>
     <row r="173" spans="1:9" ht="101.45">
       <c r="A173" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B173" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C173" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="D173" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="E173">
         <v>1</v>
       </c>
       <c r="G173" s="5" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="174" spans="1:9">
       <c r="A174" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B174" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="C174" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="D174" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="E174">
         <v>2</v>
       </c>
       <c r="G174" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="175" spans="1:9">
       <c r="A175" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B175" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C175" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D175" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="E175">
         <v>1</v>
@@ -6704,36 +6710,36 @@
     </row>
     <row r="176" spans="1:9">
       <c r="A176" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B176" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C176" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="D176" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="E176">
         <v>15</v>
       </c>
       <c r="F176" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="177" spans="1:9">
       <c r="A177" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B177" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C177" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D177" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="E177">
         <v>0</v>
@@ -6744,36 +6750,36 @@
     </row>
     <row r="178" spans="1:9">
       <c r="A178" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B178" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C178" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="D178" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="E178">
         <v>1</v>
       </c>
       <c r="F178" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="179" spans="1:9">
       <c r="A179" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B179" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C179" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="D179" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="E179">
         <v>4</v>
@@ -6784,16 +6790,16 @@
     </row>
     <row r="180" spans="1:9">
       <c r="A180" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B180" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C180" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="D180" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="E180">
         <v>1</v>
@@ -6804,36 +6810,36 @@
     </row>
     <row r="181" spans="1:9">
       <c r="A181" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B181" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C181" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="D181" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="E181">
         <v>0</v>
       </c>
       <c r="G181" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="182" spans="1:9">
       <c r="A182" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B182" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C182" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="D182" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="E182">
         <v>2</v>
@@ -6844,16 +6850,16 @@
     </row>
     <row r="183" spans="1:9">
       <c r="A183" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B183" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C183" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D183" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="E183">
         <v>3</v>
@@ -6864,79 +6870,79 @@
     </row>
     <row r="184" spans="1:9" ht="29.1">
       <c r="A184" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B184" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C184" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="D184" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E184">
         <v>2</v>
       </c>
       <c r="G184" s="5" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="I184" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="57.95">
       <c r="A185" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B185" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C185" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="D185" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="E185">
         <v>3</v>
       </c>
       <c r="G185" s="5" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="409.5">
       <c r="A186" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B186" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C186" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="D186" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="E186">
         <v>0</v>
       </c>
       <c r="G186" s="5" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="187" spans="1:9">
       <c r="A187" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B187" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="C187" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="D187" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="E187">
         <v>11</v>
@@ -6947,16 +6953,16 @@
     </row>
     <row r="188" spans="1:9">
       <c r="A188" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B188" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C188" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D188" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="E188">
         <v>2</v>
@@ -6967,16 +6973,16 @@
     </row>
     <row r="189" spans="1:9">
       <c r="A189" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B189" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C189" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="D189" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="E189">
         <v>0</v>
@@ -6987,36 +6993,36 @@
     </row>
     <row r="190" spans="1:9" ht="29.1">
       <c r="A190" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B190" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C190" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D190" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E190">
         <v>3</v>
       </c>
       <c r="G190" s="5" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="191" spans="1:9">
       <c r="A191" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B191" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C191" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="D191" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="E191">
         <v>1</v>
@@ -7027,16 +7033,16 @@
     </row>
     <row r="192" spans="1:9">
       <c r="A192" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B192" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C192" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="D192" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="E192">
         <v>7</v>
@@ -7047,16 +7053,16 @@
     </row>
     <row r="193" spans="1:8">
       <c r="A193" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B193" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C193" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="D193" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="E193">
         <v>0</v>
@@ -7067,16 +7073,16 @@
     </row>
     <row r="194" spans="1:8">
       <c r="A194" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B194" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C194" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="D194" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="E194">
         <v>9</v>
@@ -7087,16 +7093,16 @@
     </row>
     <row r="195" spans="1:8">
       <c r="A195" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B195" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C195" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="D195" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="E195">
         <v>0</v>
@@ -7107,16 +7113,16 @@
     </row>
     <row r="196" spans="1:8">
       <c r="A196" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="B196" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C196" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D196" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -7127,16 +7133,16 @@
     </row>
     <row r="197" spans="1:8">
       <c r="A197" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B197" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C197" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="D197" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="E197">
         <v>0</v>
@@ -7147,16 +7153,16 @@
     </row>
     <row r="198" spans="1:8">
       <c r="A198" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B198" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C198" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="D198" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="E198">
         <v>1</v>
@@ -7167,16 +7173,16 @@
     </row>
     <row r="199" spans="1:8">
       <c r="A199" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B199" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C199" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="D199" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="E199">
         <v>4</v>
@@ -7187,16 +7193,16 @@
     </row>
     <row r="200" spans="1:8">
       <c r="A200" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B200" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="C200" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="D200" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="E200">
         <v>2</v>
@@ -7207,16 +7213,16 @@
     </row>
     <row r="201" spans="1:8">
       <c r="A201" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B201" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C201" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="D201" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E201">
         <v>2</v>
@@ -7233,13 +7239,18 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9825220c-38e9-4650-b4a8-a5a476eee53b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f656b3e5-a944-4766-b92d-ab64d774771f" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF7374402B6A4A4EA8C2DF4C907C62CE" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="634fed6cab9e0ec94dd9098b4fe0b85b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9825220c-38e9-4650-b4a8-a5a476eee53b" xmlns:ns3="f656b3e5-a944-4766-b92d-ab64d774771f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8def64ac084b0ae7b89854ef6d0f5db3" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF7374402B6A4A4EA8C2DF4C907C62CE" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b77c5a9c7caa9b0b3fe71064a54dc07">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9825220c-38e9-4650-b4a8-a5a476eee53b" xmlns:ns3="f656b3e5-a944-4766-b92d-ab64d774771f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34ac8d575deb00ce5f342b767d038d83" ns2:_="" ns3:_="">
     <xsd:import namespace="9825220c-38e9-4650-b4a8-a5a476eee53b"/>
     <xsd:import namespace="f656b3e5-a944-4766-b92d-ab64d774771f"/>
     <xsd:element name="properties">
@@ -7260,6 +7271,8 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -7324,6 +7337,13 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="b31da6f4-e52d-49d7-b108-9c7783d77463" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f656b3e5-a944-4766-b92d-ab64d774771f" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -7353,6 +7373,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{8d14aa98-b07c-4e27-8642-7316a2cb2bf9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="f656b3e5-a944-4766-b92d-ab64d774771f">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -7468,7 +7499,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90ABD40C-6A1F-49B3-9AA8-01DED8E67C63}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38397CFA-D31C-4E39-B68C-26F60E4094D4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>